<commit_message>
Signed-off-by: STUDENT Edvinas Tkacenka <Edvinas.Tkacenka@students.ittralee.ie>
</commit_message>
<xml_diff>
--- a/Assignment 1.xlsx
+++ b/Assignment 1.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\t00216714\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\t00216714\Desktop\initials\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{209B3D6B-12A3-4A1C-8DE4-ADD48AB41F87}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7D3C18A-BE3E-4719-A6ED-6F7745F164AD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11280" windowHeight="7545" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11280" windowHeight="7545" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Assignment generation" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="135">
   <si>
     <t>z = -1</t>
   </si>
@@ -294,6 +294,156 @@
   </si>
   <si>
     <t xml:space="preserve">0.6614112   ,   -3.878549   ,   1.587259   ,   </t>
+  </si>
+  <si>
+    <t>0   ,   2   ,   0   ,   0</t>
+  </si>
+  <si>
+    <t>0   ,   0   ,   2   ,   0</t>
+  </si>
+  <si>
+    <t>4   ,   0   ,   0   ,   0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-43.9254   ,   6.330085   ,   -2.404688   ,   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">67.42641   ,   5.641258   ,   -1.067676   ,   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">-45.45341   ,   4.706264   ,   -1.252853   ,   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">-13.63861   ,   4.509456   ,   -0.8708496   ,   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">34.0836   ,   4.214244   ,   -0.2978446   ,   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">65.89841   ,   4.017437   ,   0.08415872   ,   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.7407827   ,   2.78723   ,   0.4719867   ,   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">16.64819   ,   2.688827   ,   0.6629883   ,   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">-6.899284   ,   -5.331876   ,   6.23116   ,   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">9.008118   ,   -5.43028   ,   6.422162   ,   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">-42.35094   ,   4.003266   ,   -5.65233   ,   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">69.00088   ,   3.314439   ,   -4.315319   ,   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">-43.87895   ,   2.379445   ,   -4.500495   ,   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">-12.06415   ,   2.182637   ,   -4.118492   ,   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">35.65806   ,   1.887426   ,   -3.545487   ,   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">67.47286   ,   1.690618   ,   -3.163484   ,   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.315244   ,   0.4604119   ,   -2.775656   ,   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">18.22265   ,   0.3620081   ,   -2.584654   ,   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">-5.324823   ,   -7.658694   ,   2.983517   ,   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">10.58258   ,   -7.757098   ,   3.174519   ,  </t>
+  </si>
+  <si>
+    <t>1   ,   0   ,   0   ,   -1</t>
+  </si>
+  <si>
+    <t>0   ,   1   ,   0   ,   -4</t>
+  </si>
+  <si>
+    <t>0   ,   0   ,   1   ,   3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10.58258   ,   -7.757098   ,   3.174519   ,   </t>
+  </si>
+  <si>
+    <t>3.976851   ,   0.1910017   ,   -0.09840383   ,   -1</t>
+  </si>
+  <si>
+    <t>-0.1968077   ,   1.623821   ,   1.163409   ,   -4</t>
+  </si>
+  <si>
+    <t>0.3820033   ,   -1.151835   ,   1.623821   ,   3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-10.98135   ,   6.330085   ,   -2.404688   ,   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">16.8566   ,   5.641258   ,   -1.067676   ,   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">-11.36335   ,   4.706264   ,   -1.252853   ,   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">-3.409652   ,   4.509456   ,   -0.8708496   ,   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">8.5209   ,   4.214244   ,   -0.2978446   ,   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">16.4746   ,   4.017437   ,   0.08415872   ,   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.1851957   ,   2.78723   ,   0.4719867   ,   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">4.162046   ,   2.688827   ,   0.6629883   ,   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">-1.724821   ,   -5.331876   ,   6.23116   ,   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.252029   ,   -5.43028   ,   6.422162   ,   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">-10.58773   ,   4.003266   ,   -5.65233   ,   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">17.25022   ,   3.314439   ,   -4.315319   ,   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">-10.96974   ,   2.379445   ,   -4.500495   ,   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">-3.016036   ,   2.182637   ,   -4.118492   ,   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">8.914515   ,   1.887426   ,   -3.545487   ,   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">16.86822   ,   1.690618   ,   -3.163484   ,   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.578811   ,   0.4604119   ,   -2.775656   ,   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">4.555662   ,   0.3620081   ,   -2.584654   ,   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">-1.331206   ,   -7.658694   ,   2.983517   ,   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.645645   ,   -7.757098   ,   3.174519   ,   </t>
   </si>
 </sst>
 </file>
@@ -357,7 +507,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="14">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -508,6 +658,15 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -517,7 +676,7 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -629,38 +788,44 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -849,6 +1014,372 @@
         <a:xfrm>
           <a:off x="1872155" y="3376448"/>
           <a:ext cx="3711466" cy="1238985"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1267810</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>39414</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>2496535</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>696639</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Picture 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1DAE11D2-67C3-4A5B-A5AE-365908AC62C3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="3100551" y="5314293"/>
+          <a:ext cx="1228725" cy="657225"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>7329</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>43963</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>7329</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>1502019</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="10" name="Picture 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0574DB99-9945-4369-8310-796EA967C24E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="1831733" y="6359771"/>
+          <a:ext cx="3773365" cy="1458056"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1250674</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>41413</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>2479399</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>698638</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="13" name="Picture 12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E5EA542E-EC4E-45DA-B33D-8FCC85CAAD42}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="3089413" y="8274326"/>
+          <a:ext cx="1228725" cy="657225"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>8283</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>8283</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>8283</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>595886</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="17" name="Picture 16">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1DEBABC3-58D2-487C-B1B7-09EDDB1D7536}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="7628283" y="5292587"/>
+          <a:ext cx="2733261" cy="587603"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>8283</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>1258431</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="20" name="Picture 19">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C5047B1B-FFB8-488B-A3F4-DD0266D8499F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="1847022" y="9268239"/>
+          <a:ext cx="3760304" cy="1258431"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>314740</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>887595</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>1225827</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="22" name="Picture 21">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{803D6E77-9FC1-412F-8B19-DAF9EC90D638}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="7620000" y="9582979"/>
+          <a:ext cx="2726334" cy="911087"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1193,8 +1724,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H24" sqref="H24"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1288,8 +1819,7 @@
         <v>14</v>
       </c>
       <c r="C8" s="31">
-        <f>INT((C4/10000))-5</f>
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="D8" s="31">
         <f>MOD(INT((C4/1000)),10)-4</f>
@@ -1357,7 +1887,7 @@
       </c>
       <c r="D12" s="29">
         <f>C8</f>
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="E12" s="29">
         <f>E8</f>
@@ -1408,8 +1938,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:M38"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12:E12"/>
+    <sheetView topLeftCell="A19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D24" sqref="D24:E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1433,10 +1963,10 @@
     </row>
     <row r="2" spans="3:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C2" s="5"/>
-      <c r="D2" s="37" t="s">
+      <c r="D2" s="39" t="s">
         <v>40</v>
       </c>
-      <c r="E2" s="38"/>
+      <c r="E2" s="40"/>
       <c r="F2" s="8"/>
       <c r="G2" s="4"/>
       <c r="H2" s="4"/>
@@ -1447,8 +1977,8 @@
     </row>
     <row r="3" spans="3:13" ht="111" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C3" s="5"/>
-      <c r="D3" s="41"/>
-      <c r="E3" s="47"/>
+      <c r="D3" s="37"/>
+      <c r="E3" s="38"/>
       <c r="F3" s="33"/>
       <c r="G3" s="11"/>
       <c r="H3" s="34"/>
@@ -1468,10 +1998,10 @@
     </row>
     <row r="5" spans="3:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C5" s="5"/>
-      <c r="D5" s="37" t="s">
+      <c r="D5" s="39" t="s">
         <v>13</v>
       </c>
-      <c r="E5" s="38"/>
+      <c r="E5" s="40"/>
       <c r="F5" s="8"/>
       <c r="H5" s="15"/>
       <c r="I5" s="12"/>
@@ -1480,8 +2010,8 @@
     </row>
     <row r="6" spans="3:13" ht="70.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C6" s="5"/>
-      <c r="D6" s="41"/>
-      <c r="E6" s="47"/>
+      <c r="D6" s="37"/>
+      <c r="E6" s="38"/>
       <c r="F6" s="16"/>
       <c r="G6" s="12"/>
       <c r="H6" s="15"/>
@@ -1501,10 +2031,10 @@
     </row>
     <row r="8" spans="3:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C8" s="5"/>
-      <c r="D8" s="37" t="s">
+      <c r="D8" s="39" t="s">
         <v>31</v>
       </c>
-      <c r="E8" s="38"/>
+      <c r="E8" s="40"/>
       <c r="F8" s="17"/>
       <c r="G8" s="12"/>
       <c r="H8" s="15"/>
@@ -1514,8 +2044,8 @@
     </row>
     <row r="9" spans="3:13" ht="124.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C9" s="5"/>
-      <c r="D9" s="41"/>
-      <c r="E9" s="47"/>
+      <c r="D9" s="37"/>
+      <c r="E9" s="38"/>
       <c r="F9" s="17"/>
       <c r="G9" s="12"/>
       <c r="H9" s="15"/>
@@ -1535,28 +2065,28 @@
     </row>
     <row r="11" spans="3:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C11" s="5"/>
-      <c r="D11" s="37" t="s">
+      <c r="D11" s="39" t="s">
         <v>4</v>
       </c>
-      <c r="E11" s="38"/>
+      <c r="E11" s="40"/>
       <c r="F11" s="18"/>
       <c r="G11" s="19"/>
-      <c r="H11" s="45" t="s">
+      <c r="H11" s="41" t="s">
         <v>16</v>
       </c>
-      <c r="I11" s="46"/>
+      <c r="I11" s="42"/>
       <c r="J11" s="8"/>
       <c r="L11" s="15"/>
       <c r="M11" s="12"/>
     </row>
     <row r="12" spans="3:13" ht="58.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C12" s="5"/>
-      <c r="D12" s="41"/>
-      <c r="E12" s="47"/>
+      <c r="D12" s="37"/>
+      <c r="E12" s="38"/>
       <c r="F12" s="16"/>
       <c r="G12" s="16"/>
-      <c r="H12" s="41"/>
-      <c r="I12" s="47"/>
+      <c r="H12" s="37"/>
+      <c r="I12" s="38"/>
       <c r="J12" s="16"/>
       <c r="K12" s="12"/>
       <c r="L12" s="15"/>
@@ -1576,10 +2106,10 @@
     </row>
     <row r="14" spans="3:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C14" s="5"/>
-      <c r="D14" s="37" t="s">
+      <c r="D14" s="39" t="s">
         <v>11</v>
       </c>
-      <c r="E14" s="38"/>
+      <c r="E14" s="40"/>
       <c r="F14" s="17"/>
       <c r="G14" s="12"/>
       <c r="H14" s="15"/>
@@ -1591,8 +2121,8 @@
     </row>
     <row r="15" spans="3:13" ht="121.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C15" s="5"/>
-      <c r="D15" s="41"/>
-      <c r="E15" s="47"/>
+      <c r="D15" s="37"/>
+      <c r="E15" s="38"/>
       <c r="F15" s="17"/>
       <c r="G15" s="12"/>
       <c r="H15" s="15"/>
@@ -1616,10 +2146,10 @@
     </row>
     <row r="17" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C17" s="5"/>
-      <c r="D17" s="37" t="s">
+      <c r="D17" s="39" t="s">
         <v>3</v>
       </c>
-      <c r="E17" s="38"/>
+      <c r="E17" s="40"/>
       <c r="F17" s="18"/>
       <c r="G17" s="12"/>
       <c r="H17" s="15"/>
@@ -1631,8 +2161,8 @@
     </row>
     <row r="18" spans="1:13" ht="55.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C18" s="5"/>
-      <c r="D18" s="41"/>
-      <c r="E18" s="47"/>
+      <c r="D18" s="37"/>
+      <c r="E18" s="38"/>
       <c r="F18" s="20"/>
       <c r="H18" s="15"/>
       <c r="I18" s="12"/>
@@ -1653,18 +2183,18 @@
     </row>
     <row r="20" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C20" s="5"/>
-      <c r="D20" s="37" t="s">
+      <c r="D20" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="E20" s="38"/>
-      <c r="F20" s="42" t="s">
+      <c r="E20" s="40"/>
+      <c r="F20" s="43" t="s">
         <v>33</v>
       </c>
       <c r="G20" s="44"/>
-      <c r="H20" s="45" t="s">
+      <c r="H20" s="41" t="s">
         <v>1</v>
       </c>
-      <c r="I20" s="46"/>
+      <c r="I20" s="42"/>
       <c r="J20" s="17"/>
       <c r="K20" s="12"/>
       <c r="L20" s="15"/>
@@ -1672,12 +2202,12 @@
     </row>
     <row r="21" spans="1:13" ht="114" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C21" s="5"/>
-      <c r="D21" s="41"/>
-      <c r="E21" s="47"/>
-      <c r="F21" s="42"/>
+      <c r="D21" s="37"/>
+      <c r="E21" s="38"/>
+      <c r="F21" s="43"/>
       <c r="G21" s="44"/>
-      <c r="H21" s="41"/>
-      <c r="I21" s="47"/>
+      <c r="H21" s="37"/>
+      <c r="I21" s="38"/>
       <c r="J21" s="17"/>
       <c r="K21" s="12"/>
       <c r="L21" s="15"/>
@@ -1695,33 +2225,33 @@
     </row>
     <row r="23" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C23" s="5"/>
-      <c r="D23" s="37" t="s">
+      <c r="D23" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="E23" s="38"/>
+      <c r="E23" s="40"/>
       <c r="F23" s="9"/>
       <c r="G23" s="22"/>
       <c r="H23" s="22"/>
       <c r="I23" s="22"/>
       <c r="J23" s="10"/>
       <c r="K23" s="18"/>
-      <c r="L23" s="45" t="s">
+      <c r="L23" s="41" t="s">
         <v>22</v>
       </c>
-      <c r="M23" s="46"/>
+      <c r="M23" s="42"/>
     </row>
     <row r="24" spans="1:13" ht="113.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C24" s="5"/>
-      <c r="D24" s="41"/>
-      <c r="E24" s="47"/>
+      <c r="D24" s="37"/>
+      <c r="E24" s="38"/>
       <c r="F24" s="6"/>
       <c r="G24" s="11"/>
       <c r="H24" s="11"/>
       <c r="I24" s="11"/>
       <c r="J24" s="7"/>
       <c r="K24" s="23"/>
-      <c r="L24" s="41"/>
-      <c r="M24" s="47"/>
+      <c r="L24" s="37"/>
+      <c r="M24" s="38"/>
     </row>
     <row r="25" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D25" s="13"/>
@@ -1734,10 +2264,10 @@
     <row r="26" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B26" s="4"/>
       <c r="C26" s="24"/>
-      <c r="D26" s="45" t="s">
+      <c r="D26" s="41" t="s">
         <v>18</v>
       </c>
-      <c r="E26" s="46"/>
+      <c r="E26" s="42"/>
       <c r="F26" s="12"/>
       <c r="J26" s="15"/>
       <c r="K26" s="12"/>
@@ -1748,8 +2278,8 @@
       <c r="A27" s="5"/>
       <c r="B27" s="6"/>
       <c r="C27" s="7"/>
-      <c r="D27" s="41"/>
-      <c r="E27" s="47"/>
+      <c r="D27" s="37"/>
+      <c r="E27" s="38"/>
       <c r="F27" s="12"/>
       <c r="J27" s="15"/>
       <c r="K27" s="12"/>
@@ -1767,15 +2297,15 @@
       <c r="M28" s="12"/>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A29" s="45" t="s">
+      <c r="A29" s="41" t="s">
         <v>34</v>
       </c>
-      <c r="B29" s="46"/>
+      <c r="B29" s="42"/>
       <c r="C29" s="25"/>
-      <c r="D29" s="37" t="s">
+      <c r="D29" s="39" t="s">
         <v>15</v>
       </c>
-      <c r="E29" s="38"/>
+      <c r="E29" s="40"/>
       <c r="F29" s="9"/>
       <c r="G29" s="22"/>
       <c r="H29" s="22"/>
@@ -1786,11 +2316,11 @@
       <c r="M29" s="12"/>
     </row>
     <row r="30" spans="1:13" ht="69.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="41"/>
-      <c r="B30" s="47"/>
+      <c r="A30" s="37"/>
+      <c r="B30" s="38"/>
       <c r="C30" s="25"/>
-      <c r="D30" s="41"/>
-      <c r="E30" s="47"/>
+      <c r="D30" s="37"/>
+      <c r="E30" s="38"/>
       <c r="F30" s="20"/>
       <c r="G30" s="21"/>
       <c r="H30" s="21"/>
@@ -1808,44 +2338,44 @@
       <c r="M31" s="8"/>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A32" s="37" t="s">
+      <c r="A32" s="39" t="s">
         <v>12</v>
       </c>
-      <c r="B32" s="38"/>
+      <c r="B32" s="40"/>
       <c r="C32" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="D32" s="37" t="s">
+      <c r="D32" s="39" t="s">
         <v>12</v>
       </c>
-      <c r="E32" s="38"/>
-      <c r="F32" s="42" t="s">
+      <c r="E32" s="40"/>
+      <c r="F32" s="43" t="s">
         <v>32</v>
       </c>
-      <c r="G32" s="43"/>
-      <c r="H32" s="43"/>
-      <c r="I32" s="43"/>
-      <c r="J32" s="43"/>
+      <c r="G32" s="46"/>
+      <c r="H32" s="46"/>
+      <c r="I32" s="46"/>
+      <c r="J32" s="46"/>
       <c r="K32" s="44"/>
-      <c r="L32" s="37" t="s">
+      <c r="L32" s="39" t="s">
         <v>12</v>
       </c>
-      <c r="M32" s="38"/>
+      <c r="M32" s="40"/>
     </row>
     <row r="33" spans="1:13" ht="116.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="39"/>
-      <c r="B33" s="40"/>
+      <c r="A33" s="47"/>
+      <c r="B33" s="45"/>
       <c r="C33" s="17"/>
-      <c r="D33" s="41"/>
-      <c r="E33" s="40"/>
-      <c r="F33" s="42"/>
-      <c r="G33" s="43"/>
-      <c r="H33" s="43"/>
-      <c r="I33" s="43"/>
-      <c r="J33" s="43"/>
+      <c r="D33" s="37"/>
+      <c r="E33" s="45"/>
+      <c r="F33" s="43"/>
+      <c r="G33" s="46"/>
+      <c r="H33" s="46"/>
+      <c r="I33" s="46"/>
+      <c r="J33" s="46"/>
       <c r="K33" s="44"/>
-      <c r="L33" s="41"/>
-      <c r="M33" s="40"/>
+      <c r="L33" s="37"/>
+      <c r="M33" s="45"/>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A34" s="21"/>
@@ -1857,32 +2387,47 @@
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.2">
       <c r="C35" s="5"/>
-      <c r="D35" s="45" t="s">
+      <c r="D35" s="41" t="s">
         <v>21</v>
       </c>
-      <c r="E35" s="46"/>
+      <c r="E35" s="42"/>
       <c r="F35" s="12"/>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.2">
       <c r="C36" s="5"/>
-      <c r="D36" s="41"/>
-      <c r="E36" s="47"/>
+      <c r="D36" s="37"/>
+      <c r="E36" s="38"/>
       <c r="F36" s="12"/>
     </row>
     <row r="38" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E38" s="26"/>
       <c r="F38" s="26"/>
-      <c r="H38" s="41"/>
-      <c r="I38" s="40"/>
+      <c r="H38" s="37"/>
+      <c r="I38" s="45"/>
     </row>
   </sheetData>
   <mergeCells count="41">
-    <mergeCell ref="D9:E9"/>
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="L32:M32"/>
+    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="D33:E33"/>
+    <mergeCell ref="F33:K33"/>
+    <mergeCell ref="L33:M33"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="D32:E32"/>
+    <mergeCell ref="D35:E35"/>
+    <mergeCell ref="H38:I38"/>
+    <mergeCell ref="D36:E36"/>
+    <mergeCell ref="F32:K32"/>
+    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="D29:E29"/>
+    <mergeCell ref="D27:E27"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="D30:E30"/>
+    <mergeCell ref="D23:E23"/>
+    <mergeCell ref="L23:M23"/>
+    <mergeCell ref="D24:E24"/>
+    <mergeCell ref="L24:M24"/>
+    <mergeCell ref="D26:E26"/>
     <mergeCell ref="H20:I20"/>
     <mergeCell ref="D21:E21"/>
     <mergeCell ref="F21:G21"/>
@@ -1897,27 +2442,12 @@
     <mergeCell ref="D18:E18"/>
     <mergeCell ref="D20:E20"/>
     <mergeCell ref="F20:G20"/>
-    <mergeCell ref="D27:E27"/>
-    <mergeCell ref="A30:B30"/>
-    <mergeCell ref="D30:E30"/>
-    <mergeCell ref="D23:E23"/>
-    <mergeCell ref="L23:M23"/>
-    <mergeCell ref="D24:E24"/>
-    <mergeCell ref="L24:M24"/>
-    <mergeCell ref="D26:E26"/>
-    <mergeCell ref="D35:E35"/>
-    <mergeCell ref="H38:I38"/>
-    <mergeCell ref="D36:E36"/>
-    <mergeCell ref="F32:K32"/>
-    <mergeCell ref="A29:B29"/>
-    <mergeCell ref="D29:E29"/>
-    <mergeCell ref="L32:M32"/>
-    <mergeCell ref="A33:B33"/>
-    <mergeCell ref="D33:E33"/>
-    <mergeCell ref="F33:K33"/>
-    <mergeCell ref="L33:M33"/>
-    <mergeCell ref="A32:B32"/>
-    <mergeCell ref="D32:E32"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="D8:E8"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -1928,15 +2458,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41D60858-96FD-428D-BE82-69C1DB933610}">
-  <dimension ref="A1:I29"/>
+  <dimension ref="A1:T69"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E11" sqref="E11:L20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="W12" sqref="W12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>41</v>
       </c>
@@ -1950,7 +2480,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>42</v>
       </c>
@@ -1964,7 +2494,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>43</v>
       </c>
@@ -1978,7 +2508,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>44</v>
       </c>
@@ -1992,7 +2522,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>45</v>
       </c>
@@ -2006,39 +2536,65 @@
         <v>60</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>109</v>
+      </c>
       <c r="E11" t="s">
         <v>65</v>
       </c>
       <c r="I11" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="N11" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>110</v>
+      </c>
       <c r="E12" t="s">
         <v>66</v>
       </c>
       <c r="I12" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="N12" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>64</v>
+      </c>
       <c r="E13" t="s">
         <v>67</v>
       </c>
       <c r="I13" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="N13" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="E14" t="s">
         <v>68</v>
       </c>
       <c r="I14" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="N14" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
       <c r="E15" t="s">
         <v>69</v>
       </c>
@@ -2046,7 +2602,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
       <c r="E16" t="s">
         <v>70</v>
       </c>
@@ -2054,7 +2610,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="17" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:13" x14ac:dyDescent="0.2">
       <c r="E17" t="s">
         <v>71</v>
       </c>
@@ -2062,7 +2618,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="18" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:13" x14ac:dyDescent="0.2">
       <c r="E18" t="s">
         <v>72</v>
       </c>
@@ -2070,7 +2626,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="19" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:13" x14ac:dyDescent="0.2">
       <c r="E19" t="s">
         <v>73</v>
       </c>
@@ -2078,7 +2634,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="20" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:13" x14ac:dyDescent="0.2">
       <c r="E20" t="s">
         <v>74</v>
       </c>
@@ -2086,28 +2642,451 @@
         <v>84</v>
       </c>
     </row>
-    <row r="26" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B26" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="27" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B27" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="28" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B28" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="29" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B29" t="s">
         <v>64</v>
       </c>
     </row>
+    <row r="30" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="I30" t="s">
+        <v>88</v>
+      </c>
+      <c r="M30" s="48" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="31" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="I31" t="s">
+        <v>89</v>
+      </c>
+      <c r="M31" s="48" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="32" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="I32" t="s">
+        <v>90</v>
+      </c>
+      <c r="M32" s="48" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="33" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="I33" t="s">
+        <v>91</v>
+      </c>
+      <c r="M33" s="48" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="34" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="I34" t="s">
+        <v>92</v>
+      </c>
+      <c r="M34" s="48" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="35" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="I35" t="s">
+        <v>93</v>
+      </c>
+      <c r="M35" s="48" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="36" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="I36" t="s">
+        <v>94</v>
+      </c>
+      <c r="M36" s="48" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="37" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="I37" t="s">
+        <v>95</v>
+      </c>
+      <c r="M37" s="48" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="38" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="I38" t="s">
+        <v>96</v>
+      </c>
+      <c r="M38" s="48" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="39" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="I39" t="s">
+        <v>97</v>
+      </c>
+      <c r="M39" s="48" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="40" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="B40" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="41" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="B41" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="42" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="B42" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="43" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="B43" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="46" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>98</v>
+      </c>
+      <c r="E46" s="48" t="s">
+        <v>88</v>
+      </c>
+      <c r="F46" s="49"/>
+      <c r="G46" s="49"/>
+      <c r="H46" s="49"/>
+    </row>
+    <row r="47" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>99</v>
+      </c>
+      <c r="E47" s="48" t="s">
+        <v>89</v>
+      </c>
+      <c r="F47" s="49"/>
+      <c r="G47" s="49"/>
+      <c r="H47" s="49"/>
+      <c r="M47" t="s">
+        <v>115</v>
+      </c>
+      <c r="Q47" s="48" t="s">
+        <v>125</v>
+      </c>
+      <c r="R47" s="49"/>
+      <c r="S47" s="49"/>
+      <c r="T47" s="49"/>
+    </row>
+    <row r="48" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>100</v>
+      </c>
+      <c r="E48" s="48" t="s">
+        <v>90</v>
+      </c>
+      <c r="F48" s="49"/>
+      <c r="G48" s="49"/>
+      <c r="H48" s="49"/>
+      <c r="M48" t="s">
+        <v>116</v>
+      </c>
+      <c r="Q48" s="48" t="s">
+        <v>126</v>
+      </c>
+      <c r="R48" s="49"/>
+      <c r="S48" s="49"/>
+      <c r="T48" s="49"/>
+    </row>
+    <row r="49" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>101</v>
+      </c>
+      <c r="E49" s="48" t="s">
+        <v>91</v>
+      </c>
+      <c r="F49" s="49"/>
+      <c r="G49" s="49"/>
+      <c r="H49" s="49"/>
+      <c r="M49" t="s">
+        <v>117</v>
+      </c>
+      <c r="Q49" s="48" t="s">
+        <v>127</v>
+      </c>
+      <c r="R49" s="49"/>
+      <c r="S49" s="49"/>
+      <c r="T49" s="49"/>
+    </row>
+    <row r="50" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>102</v>
+      </c>
+      <c r="E50" s="48" t="s">
+        <v>92</v>
+      </c>
+      <c r="F50" s="49"/>
+      <c r="G50" s="49"/>
+      <c r="H50" s="49"/>
+      <c r="M50" t="s">
+        <v>118</v>
+      </c>
+      <c r="Q50" s="48" t="s">
+        <v>128</v>
+      </c>
+      <c r="R50" s="49"/>
+      <c r="S50" s="49"/>
+      <c r="T50" s="49"/>
+    </row>
+    <row r="51" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>103</v>
+      </c>
+      <c r="E51" s="48" t="s">
+        <v>93</v>
+      </c>
+      <c r="F51" s="49"/>
+      <c r="G51" s="49"/>
+      <c r="H51" s="49"/>
+      <c r="M51" t="s">
+        <v>119</v>
+      </c>
+      <c r="Q51" s="48" t="s">
+        <v>129</v>
+      </c>
+      <c r="R51" s="49"/>
+      <c r="S51" s="49"/>
+      <c r="T51" s="49"/>
+    </row>
+    <row r="52" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>104</v>
+      </c>
+      <c r="E52" s="48" t="s">
+        <v>94</v>
+      </c>
+      <c r="F52" s="49"/>
+      <c r="G52" s="49"/>
+      <c r="H52" s="49"/>
+      <c r="M52" t="s">
+        <v>120</v>
+      </c>
+      <c r="Q52" s="48" t="s">
+        <v>130</v>
+      </c>
+      <c r="R52" s="49"/>
+      <c r="S52" s="49"/>
+      <c r="T52" s="49"/>
+    </row>
+    <row r="53" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
+        <v>105</v>
+      </c>
+      <c r="E53" s="48" t="s">
+        <v>95</v>
+      </c>
+      <c r="F53" s="49"/>
+      <c r="G53" s="49"/>
+      <c r="H53" s="49"/>
+      <c r="M53" t="s">
+        <v>121</v>
+      </c>
+      <c r="Q53" s="48" t="s">
+        <v>131</v>
+      </c>
+      <c r="R53" s="49"/>
+      <c r="S53" s="49"/>
+      <c r="T53" s="49"/>
+    </row>
+    <row r="54" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>106</v>
+      </c>
+      <c r="E54" s="48" t="s">
+        <v>96</v>
+      </c>
+      <c r="F54" s="49"/>
+      <c r="G54" s="49"/>
+      <c r="H54" s="49"/>
+      <c r="M54" t="s">
+        <v>122</v>
+      </c>
+      <c r="Q54" s="48" t="s">
+        <v>132</v>
+      </c>
+      <c r="R54" s="49"/>
+      <c r="S54" s="49"/>
+      <c r="T54" s="49"/>
+    </row>
+    <row r="55" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
+        <v>111</v>
+      </c>
+      <c r="E55" s="48" t="s">
+        <v>97</v>
+      </c>
+      <c r="F55" s="49"/>
+      <c r="G55" s="49"/>
+      <c r="H55" s="49"/>
+      <c r="M55" t="s">
+        <v>123</v>
+      </c>
+      <c r="Q55" s="48" t="s">
+        <v>133</v>
+      </c>
+      <c r="R55" s="49"/>
+      <c r="S55" s="49"/>
+      <c r="T55" s="49"/>
+    </row>
+    <row r="56" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="M56" t="s">
+        <v>124</v>
+      </c>
+      <c r="Q56" s="48" t="s">
+        <v>134</v>
+      </c>
+      <c r="R56" s="49"/>
+      <c r="S56" s="49"/>
+      <c r="T56" s="49"/>
+    </row>
+    <row r="60" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="C60" t="s">
+        <v>115</v>
+      </c>
+      <c r="G60" s="48" t="s">
+        <v>125</v>
+      </c>
+      <c r="H60" s="49"/>
+      <c r="I60" s="49"/>
+      <c r="J60" s="49"/>
+      <c r="K60" s="49"/>
+    </row>
+    <row r="61" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="C61" t="s">
+        <v>116</v>
+      </c>
+      <c r="G61" s="48" t="s">
+        <v>126</v>
+      </c>
+      <c r="H61" s="49"/>
+      <c r="I61" s="49"/>
+      <c r="J61" s="49"/>
+      <c r="K61" s="49"/>
+    </row>
+    <row r="62" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="C62" t="s">
+        <v>117</v>
+      </c>
+      <c r="G62" s="48" t="s">
+        <v>127</v>
+      </c>
+      <c r="H62" s="49"/>
+      <c r="I62" s="49"/>
+      <c r="J62" s="49"/>
+      <c r="K62" s="49"/>
+    </row>
+    <row r="63" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="C63" t="s">
+        <v>118</v>
+      </c>
+      <c r="G63" s="48" t="s">
+        <v>128</v>
+      </c>
+      <c r="H63" s="49"/>
+      <c r="I63" s="49"/>
+      <c r="J63" s="49"/>
+      <c r="K63" s="49"/>
+    </row>
+    <row r="64" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="C64" t="s">
+        <v>119</v>
+      </c>
+      <c r="G64" s="48" t="s">
+        <v>129</v>
+      </c>
+      <c r="H64" s="49"/>
+      <c r="I64" s="49"/>
+      <c r="J64" s="49"/>
+      <c r="K64" s="49"/>
+    </row>
+    <row r="65" spans="3:11" x14ac:dyDescent="0.2">
+      <c r="C65" t="s">
+        <v>120</v>
+      </c>
+      <c r="G65" s="48" t="s">
+        <v>130</v>
+      </c>
+      <c r="H65" s="49"/>
+      <c r="I65" s="49"/>
+      <c r="J65" s="49"/>
+      <c r="K65" s="49"/>
+    </row>
+    <row r="66" spans="3:11" x14ac:dyDescent="0.2">
+      <c r="C66" t="s">
+        <v>121</v>
+      </c>
+      <c r="G66" s="48" t="s">
+        <v>131</v>
+      </c>
+      <c r="H66" s="49"/>
+      <c r="I66" s="49"/>
+      <c r="J66" s="49"/>
+      <c r="K66" s="49"/>
+    </row>
+    <row r="67" spans="3:11" x14ac:dyDescent="0.2">
+      <c r="C67" t="s">
+        <v>122</v>
+      </c>
+      <c r="G67" s="48" t="s">
+        <v>132</v>
+      </c>
+      <c r="H67" s="49"/>
+      <c r="I67" s="49"/>
+      <c r="J67" s="49"/>
+      <c r="K67" s="49"/>
+    </row>
+    <row r="68" spans="3:11" x14ac:dyDescent="0.2">
+      <c r="C68" t="s">
+        <v>123</v>
+      </c>
+      <c r="G68" s="48" t="s">
+        <v>133</v>
+      </c>
+      <c r="H68" s="49"/>
+      <c r="I68" s="49"/>
+      <c r="J68" s="49"/>
+      <c r="K68" s="49"/>
+    </row>
+    <row r="69" spans="3:11" x14ac:dyDescent="0.2">
+      <c r="C69" t="s">
+        <v>124</v>
+      </c>
+      <c r="G69" s="48" t="s">
+        <v>134</v>
+      </c>
+      <c r="H69" s="49"/>
+      <c r="I69" s="49"/>
+      <c r="J69" s="49"/>
+      <c r="K69" s="49"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>